<commit_message>
Tests adjusted to latest examples
</commit_message>
<xml_diff>
--- a/tests/files/ExcelTest4.ipynb.xlsx
+++ b/tests/files/ExcelTest4.ipynb.xlsx
@@ -156,7 +156,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>51923</xdr:colOff>
+      <xdr:colOff>1111</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>102404</xdr:rowOff>
     </xdr:to>
@@ -176,7 +176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="2857500"/>
-          <a:ext cx="4928723" cy="3531404"/>
+          <a:ext cx="4877911" cy="3531404"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -522,16 +522,16 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>-0.180021</v>
+        <v>1.764052</v>
       </c>
       <c r="D8">
-        <v>0.353262</v>
+        <v>0.400157</v>
       </c>
       <c r="E8">
-        <v>0.09273199999999999</v>
+        <v>0.978738</v>
       </c>
       <c r="F8">
-        <v>1.307977</v>
+        <v>2.240893</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -539,16 +539,16 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>1.685297</v>
+        <v>1.867558</v>
       </c>
       <c r="D9">
-        <v>1.224822</v>
+        <v>-0.977278</v>
       </c>
       <c r="E9">
-        <v>-0.633752</v>
+        <v>0.950088</v>
       </c>
       <c r="F9">
-        <v>0.469845</v>
+        <v>-0.151357</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -556,16 +556,16 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>-0.758091</v>
+        <v>-0.103219</v>
       </c>
       <c r="D10">
-        <v>-2.011591</v>
+        <v>0.410599</v>
       </c>
       <c r="E10">
-        <v>0.007983000000000001</v>
+        <v>0.144044</v>
       </c>
       <c r="F10">
-        <v>-0.232754</v>
+        <v>1.454274</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -573,16 +573,16 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1.210486</v>
+        <v>0.761038</v>
       </c>
       <c r="D11">
-        <v>0.727872</v>
+        <v>0.121675</v>
       </c>
       <c r="E11">
-        <v>-0.178372</v>
+        <v>0.443863</v>
       </c>
       <c r="F11">
-        <v>-1.008124</v>
+        <v>0.333674</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -590,16 +590,16 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>-0.345644</v>
+        <v>1.494079</v>
       </c>
       <c r="D12">
-        <v>-0.483128</v>
+        <v>-0.205158</v>
       </c>
       <c r="E12">
-        <v>0.109403</v>
+        <v>0.313068</v>
       </c>
       <c r="F12">
-        <v>0.362049</v>
+        <v>-0.854096</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -607,16 +607,16 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0.697037</v>
+        <v>-2.55299</v>
       </c>
       <c r="D13">
-        <v>0.033166</v>
+        <v>0.653619</v>
       </c>
       <c r="E13">
-        <v>-0.021461</v>
+        <v>0.864436</v>
       </c>
       <c r="F13">
-        <v>1.473813</v>
+        <v>-0.742165</v>
       </c>
     </row>
     <row r="15" spans="1:6">

</xml_diff>

<commit_message>
Prepare for 0.1.6 release
</commit_message>
<xml_diff>
--- a/tests/files/ExcelTest4.ipynb.xlsx
+++ b/tests/files/ExcelTest4.ipynb.xlsx
@@ -97,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +107,14 @@
     </font>
     <font>
       <sz val="25"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -133,9 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,21 +513,22 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8">
@@ -535,7 +545,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -552,7 +562,7 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10">
@@ -569,7 +579,7 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11">
@@ -586,7 +596,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12">
@@ -603,7 +613,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C13">

</xml_diff>